<commit_message>
Stage 1: update companies data
</commit_message>
<xml_diff>
--- a/docs/assets/data/master_companies.xlsx
+++ b/docs/assets/data/master_companies.xlsx
@@ -538,12 +538,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RESONANCE TECHNOLOGIES LTD</t>
+          <t>NIKKOLEE LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16473822</t>
+          <t>SC849775</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>71129</t>
+          <t>18110,58110,58130</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -583,12 +583,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CRAWFORD HS LIMITED</t>
+          <t>NIVADO SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16473818</t>
+          <t>16473521</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>74909</t>
+          <t>41202</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -628,12 +628,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BDL NORTH PARTNERS LTD</t>
+          <t>DARCYBROOK LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16473813</t>
+          <t>16473587</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -659,12 +659,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>68320</t>
+          <t>78109</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -673,12 +673,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ANT CARS LTD</t>
+          <t>MWB RENEWABLES LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16473814</t>
+          <t>16473843</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>49320</t>
+          <t>33190</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -718,12 +718,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PURPLE LAVENDER SERVICES LTD</t>
+          <t>PANOLUX CREATIVE LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16473825</t>
+          <t>16473840</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>86900</t>
+          <t>74202</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -763,12 +763,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SOULMATEEN LTD</t>
+          <t>A JOLLY DIME LIMITED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16473493</t>
+          <t>16473846</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -799,7 +799,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>46160,46190</t>
+          <t>56102</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -808,12 +808,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TAMWORTH GARAGE LTD</t>
+          <t>OFFICIALNEPTUNETRADING LIMITED</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16473498</t>
+          <t>16473795</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -844,7 +844,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>45200</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -853,12 +853,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JCD ROOFS LIMITED</t>
+          <t>ROLLERCOASTER BUILDING COMPANY LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16473495</t>
+          <t>16473798</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>43910</t>
+          <t>41100</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -898,12 +898,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>VILA BRITTAIN MANAGEMENT SERVICES LTD</t>
+          <t>EXPLORE THERAPY LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16473534</t>
+          <t>16473794</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>99999</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -943,12 +943,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NALLA PROPERTIES LTD</t>
+          <t>AARM RELIABLE LIMITED</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16473538</t>
+          <t>16473680</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>68100,68201,68209,68320</t>
+          <t>56210</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -988,12 +988,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>JEVOIR LTD</t>
+          <t>BUNCE E-COMMERCE LIMITED</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16473540</t>
+          <t>16473683</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>47710</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -1033,12 +1033,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LONDON PROPERTY SERVICES (BMR) LTD</t>
+          <t>GTS ACCOUNTANCY LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16473763</t>
+          <t>16473686</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>81100</t>
+          <t>69201</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -1078,12 +1078,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>KNOLA LTD</t>
+          <t>JUSTGOTYOU LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16473764</t>
+          <t>16473542</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>47910,74100</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -1123,12 +1123,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AXELFIT SYSTEMS LTD</t>
+          <t>MUHAMMAD HAMZA LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16473762</t>
+          <t>16473685</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>33200,42990,43290</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -1168,12 +1168,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CARDIUM CONSULTANCY LTD</t>
+          <t>ONLYVANS GROUP LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16473858</t>
+          <t>16473675</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>49410,49420</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -1213,12 +1213,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BEHIND THE GLASS WINDOWS, DOORS &amp; GLAZING LTD</t>
+          <t>NK.SARANG LIMITED</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16473852</t>
+          <t>16473677</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>43342</t>
+          <t>46499</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -1258,12 +1258,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>REBUILD FITNESS &amp; WELLNESS LTD</t>
+          <t>GENCO REALTY LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16473851</t>
+          <t>SC849765</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>93130</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1303,12 +1303,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NEXCHAIN TECHNOLOGIES LTD</t>
+          <t>AESTHETIC STUDIOS LONDON LTD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16473847</t>
+          <t>16473630</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>62012</t>
+          <t>59112,74201,90030</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -1348,12 +1348,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>N.K. PROPERTY SOLUTIONS LTD</t>
+          <t>INFUSION DANCE LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16473848</t>
+          <t>SC849766</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>55209,68209,68310,87900</t>
+          <t>85510</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -1393,12 +1393,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NAE BAD SPUD LTD</t>
+          <t>BURE VALLEY PROPERTY LIMITED</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SC849792</t>
+          <t>16473632</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>56103</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -1438,12 +1438,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BACALUTAPROPERTYSOLUTION LTD</t>
+          <t>STUDIO TRUE NORTH LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16473482</t>
+          <t>16473631</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>55209,68209,68320</t>
+          <t>96020</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
@@ -1483,12 +1483,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TRUE POLYGON HOLDINGS LTD</t>
+          <t>TREACLE RIGGING LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SC849753</t>
+          <t>16473633</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>43991</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
@@ -1528,12 +1528,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SHYFTABLE LTD</t>
+          <t>MOSSWOOD PROPERTY LIMITED</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16473820</t>
+          <t>16473592</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>86900</t>
+          <t>55100</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
@@ -1573,12 +1573,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MJE FACILITIES CONSULTANCY LTD</t>
+          <t>BOON AFRO-CARIBBEAN HAIR LOUNGE LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16473821</t>
+          <t>16473551</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>81100</t>
+          <t>47789</t>
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
@@ -1618,12 +1618,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FJ COURIERS LIMITED</t>
+          <t>JULIAN FRANCIS LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16473483</t>
+          <t>16473523</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>82920</t>
+          <t>38320</t>
         </is>
       </c>
       <c r="J27" t="inlineStr"/>
@@ -1663,12 +1663,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NA GLOBAL LIMITED</t>
+          <t>DAILY DASH STORE LIMITED</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16473758</t>
+          <t>16473569</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>41201,41202</t>
+          <t>47110</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
@@ -1708,12 +1708,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SSMARTTEC LTD</t>
+          <t>IACO PROPERTY LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16473466</t>
+          <t>SC849759</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>61200,62020</t>
+          <t>68100,68209</t>
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
@@ -1753,12 +1753,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>VICTORY NINE LTD</t>
+          <t>RESONANCE TECHNOLOGIES LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16473475</t>
+          <t>16473822</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>73110</t>
+          <t>71129</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
@@ -1798,12 +1798,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MIGHTY FORTRESS ESTATES LTD</t>
+          <t>DELAN CUILEY LIMITED</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16473513</t>
+          <t>NI729778</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>46210,46341,47910</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
@@ -1843,12 +1843,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>HOLLY LARKHAM CARE LTD</t>
+          <t>DISTINGUISH SISTERS LIMITED LIMITED</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16473517</t>
+          <t>16473470</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1879,7 +1879,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>87300</t>
+          <t>84120,86900,87200</t>
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
@@ -1888,12 +1888,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GANDER INVESTMENTS LTD</t>
+          <t>ROUSE SHARP LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16473515</t>
+          <t>16473550</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1919,12 +1919,12 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>68100,68209</t>
+          <t>41100,68209</t>
         </is>
       </c>
       <c r="J33" t="inlineStr"/>
@@ -1933,12 +1933,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GLOBAL LETTING AND MAINTENANCE LTD</t>
+          <t>RUGER CONSULTING LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16473561</t>
+          <t>16473547</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
@@ -1978,12 +1978,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ROKSEE LIMITED</t>
+          <t>SDT GLOBAL SERVICES LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16473563</t>
+          <t>16473808</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>47190,69201,70229,71122</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
@@ -2023,12 +2023,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ZENCRUITERS LTD</t>
+          <t>NFGU COACHING LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16473562</t>
+          <t>16473802</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2059,7 +2059,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>78109</t>
+          <t>93130</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
@@ -2068,12 +2068,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>COMPASS HOUSING SOLUTIONS LTD</t>
+          <t>ZEENUNGOS LIMITED</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16473554</t>
+          <t>16473674</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>87100</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -2113,12 +2113,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>HIGH STREET CORNER STORE LTD</t>
+          <t>LAYLAH COUNSELLING LIMITED</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16473558</t>
+          <t>16473672</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>47110</t>
+          <t>84120</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -2158,12 +2158,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>RESOLUTIO CONSULTING LTD</t>
+          <t>THE BUNKER LEVEN LIMITED</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16473560</t>
+          <t>SC849768</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>82990</t>
+          <t>56302</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
@@ -2203,12 +2203,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TAP &amp; WASH LTD</t>
+          <t>EN4 RESTAURANT LIMITED</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16473555</t>
+          <t>16473650</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2239,7 +2239,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>81299</t>
+          <t>56101</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
@@ -2248,12 +2248,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SEVEN (HOLDCO) LIMITED</t>
+          <t>LATHAM INDUSTRIES (WEST MIDLANDS) LIMITED</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16473606</t>
+          <t>16473643</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2284,29 +2284,21 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>64209</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>Activities of other holding companies n.e.c.</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
-        </is>
-      </c>
+          <t>31090</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CLARITY HOME HUB HEALTH LTD</t>
+          <t>SELDUR LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16473605</t>
+          <t>16473642</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2337,7 +2329,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>86900</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
@@ -2346,12 +2338,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>FHFC LIMITED</t>
+          <t>PITU BRICKWORK LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16473652</t>
+          <t>16473644</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2382,7 +2374,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>41202</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
@@ -2391,12 +2383,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MZOF LTD</t>
+          <t>HOUSE OF SAFFRON LIMITED</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16473719</t>
+          <t>16473645</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2427,7 +2419,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>59111</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J44" t="inlineStr"/>
@@ -2436,12 +2428,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ECOPOWER RENEWABLE SOLUTIONS LTD</t>
+          <t>ELMWOOD PROPERTY MANAGEMENT AND LETTINGS LIMITED</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SC849780</t>
+          <t>16473574</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2472,7 +2464,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>43210</t>
+          <t>68209,68320</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
@@ -2481,12 +2473,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R&amp;H KHUSHI LTD</t>
+          <t>WOW BUBBLES BARNSLEY LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16473718</t>
+          <t>16473572</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2517,7 +2509,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>56102</t>
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
@@ -2526,12 +2518,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MURRAY'S COFFEE LTD</t>
+          <t>NOTHING SOUNDS GOOD LIMITED</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16473717</t>
+          <t>16473566</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2562,7 +2554,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>10832,56103,56210</t>
+          <t>47630</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -2571,12 +2563,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MINI PRINT FACTORY LTD</t>
+          <t>SAGA STUDIO LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16473759</t>
+          <t>16473564</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2607,7 +2599,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>74100</t>
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
@@ -2616,12 +2608,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>WELCOME MART LTD</t>
+          <t>BURY LODGE FARM &amp; SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16473757</t>
+          <t>16473568</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2652,7 +2644,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>01300,01500</t>
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
@@ -2661,12 +2653,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>EL RESALES LTD</t>
+          <t>AEVA MEDICAL LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SC849752</t>
+          <t>16473575</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2697,7 +2689,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>86220,86900,96020</t>
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
@@ -2706,12 +2698,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>GD PROPERTY GROUP LIMITED</t>
+          <t>WWFD CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16473525</t>
+          <t>16473591</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2742,7 +2734,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>68100</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
@@ -2751,12 +2743,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>J&amp;F STUDIOS LTD</t>
+          <t>JAMBURI LTD</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16473474</t>
+          <t>16473543</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2787,7 +2779,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>74201,74209</t>
+          <t>56103</t>
         </is>
       </c>
       <c r="J52" t="inlineStr"/>
@@ -2796,12 +2788,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>JUSTGOTYOU LTD</t>
+          <t>J&amp;F STUDIOS LTD</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16473542</t>
+          <t>16473474</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2832,7 +2824,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>47910,74100</t>
+          <t>74201,74209</t>
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
@@ -2841,12 +2833,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>WWFD CONSULTING LIMITED</t>
+          <t>KNOLA LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16473591</t>
+          <t>16473764</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2877,7 +2869,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J54" t="inlineStr"/>
@@ -2886,12 +2878,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>MOSSWOOD PROPERTY LIMITED</t>
+          <t>SHYFTABLE LTD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16473592</t>
+          <t>16473820</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2922,7 +2914,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>55100</t>
+          <t>86900</t>
         </is>
       </c>
       <c r="J55" t="inlineStr"/>
@@ -2931,12 +2923,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>TREACLE RIGGING LTD</t>
+          <t>TRUE POLYGON HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16473633</t>
+          <t>SC849753</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2967,7 +2959,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>43991</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J56" t="inlineStr"/>
@@ -2976,12 +2968,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>STUDIO TRUE NORTH LTD</t>
+          <t>BACALUTAPROPERTYSOLUTION LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16473631</t>
+          <t>16473482</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3012,7 +3004,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>96020</t>
+          <t>55209,68209,68320</t>
         </is>
       </c>
       <c r="J57" t="inlineStr"/>
@@ -3021,12 +3013,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BURE VALLEY PROPERTY LIMITED</t>
+          <t>NAE BAD SPUD LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16473632</t>
+          <t>SC849792</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3057,7 +3049,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>56103</t>
         </is>
       </c>
       <c r="J58" t="inlineStr"/>
@@ -3066,12 +3058,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>INFUSION DANCE LTD</t>
+          <t>N.K. PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SC849766</t>
+          <t>16473848</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3102,7 +3094,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>85510</t>
+          <t>55209,68209,68310,87900</t>
         </is>
       </c>
       <c r="J59" t="inlineStr"/>
@@ -3111,12 +3103,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>AESTHETIC STUDIOS LONDON LTD</t>
+          <t>NEXCHAIN TECHNOLOGIES LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16473630</t>
+          <t>16473847</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3147,7 +3139,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>59112,74201,90030</t>
+          <t>62012</t>
         </is>
       </c>
       <c r="J60" t="inlineStr"/>
@@ -3156,12 +3148,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>GENCO REALTY LTD</t>
+          <t>REBUILD FITNESS &amp; WELLNESS LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>SC849765</t>
+          <t>16473851</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3192,7 +3184,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>93130</t>
         </is>
       </c>
       <c r="J61" t="inlineStr"/>
@@ -3201,12 +3193,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>NK.SARANG LIMITED</t>
+          <t>BEHIND THE GLASS WINDOWS, DOORS &amp; GLAZING LTD</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16473677</t>
+          <t>16473852</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3237,7 +3229,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>46499</t>
+          <t>43342</t>
         </is>
       </c>
       <c r="J62" t="inlineStr"/>
@@ -3246,12 +3238,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>ONLYVANS GROUP LTD</t>
+          <t>CARDIUM CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16473675</t>
+          <t>16473858</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3282,7 +3274,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>49410,49420</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J63" t="inlineStr"/>
@@ -3291,12 +3283,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>MUHAMMAD HAMZA LTD</t>
+          <t>AXELFIT SYSTEMS LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16473685</t>
+          <t>16473762</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3327,7 +3319,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>33200,42990,43290</t>
         </is>
       </c>
       <c r="J64" t="inlineStr"/>
@@ -3336,12 +3328,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>GTS ACCOUNTANCY LTD</t>
+          <t>LONDON PROPERTY SERVICES (BMR) LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16473686</t>
+          <t>16473763</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3372,7 +3364,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>69201</t>
+          <t>81100</t>
         </is>
       </c>
       <c r="J65" t="inlineStr"/>
@@ -3381,12 +3373,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>NIKKOLEE LTD</t>
+          <t>FJ COURIERS LIMITED</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>SC849775</t>
+          <t>16473483</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3417,7 +3409,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>18110,58110,58130</t>
+          <t>82920</t>
         </is>
       </c>
       <c r="J66" t="inlineStr"/>
@@ -3426,12 +3418,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BUNCE E-COMMERCE LIMITED</t>
+          <t>JEVOIR LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16473683</t>
+          <t>16473540</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3462,7 +3454,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>47710</t>
         </is>
       </c>
       <c r="J67" t="inlineStr"/>
@@ -3471,12 +3463,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>AARM RELIABLE LIMITED</t>
+          <t>NALLA PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16473680</t>
+          <t>16473538</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3507,7 +3499,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>56210</t>
+          <t>68100,68201,68209,68320</t>
         </is>
       </c>
       <c r="J68" t="inlineStr"/>
@@ -3516,12 +3508,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>EXPLORE THERAPY LTD</t>
+          <t>VILA BRITTAIN MANAGEMENT SERVICES LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16473794</t>
+          <t>16473534</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3552,7 +3544,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>99999</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J69" t="inlineStr"/>
@@ -3561,12 +3553,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ROLLERCOASTER BUILDING COMPANY LTD</t>
+          <t>JCD ROOFS LIMITED</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16473798</t>
+          <t>16473495</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3597,7 +3589,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>41100</t>
+          <t>43910</t>
         </is>
       </c>
       <c r="J70" t="inlineStr"/>
@@ -3606,12 +3598,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>OFFICIALNEPTUNETRADING LIMITED</t>
+          <t>TAMWORTH GARAGE LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16473795</t>
+          <t>16473498</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3642,7 +3634,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>45200</t>
         </is>
       </c>
       <c r="J71" t="inlineStr"/>
@@ -3651,12 +3643,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>A JOLLY DIME LIMITED</t>
+          <t>SOULMATEEN LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16473846</t>
+          <t>16473493</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3687,7 +3679,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>56102</t>
+          <t>46160,46190</t>
         </is>
       </c>
       <c r="J72" t="inlineStr"/>
@@ -3696,12 +3688,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>PANOLUX CREATIVE LTD</t>
+          <t>PURPLE LAVENDER SERVICES LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16473840</t>
+          <t>16473825</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3732,7 +3724,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>74202</t>
+          <t>86900</t>
         </is>
       </c>
       <c r="J73" t="inlineStr"/>
@@ -3741,12 +3733,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MWB RENEWABLES LTD</t>
+          <t>ANT CARS LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16473843</t>
+          <t>16473814</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3777,7 +3769,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>33190</t>
+          <t>49320</t>
         </is>
       </c>
       <c r="J74" t="inlineStr"/>
@@ -3786,12 +3778,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>DARCYBROOK LTD</t>
+          <t>BDL NORTH PARTNERS LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16473587</t>
+          <t>16473813</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3817,12 +3809,12 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>78109</t>
+          <t>68320</t>
         </is>
       </c>
       <c r="J75" t="inlineStr"/>
@@ -3831,12 +3823,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>JAMBURI LTD</t>
+          <t>GD PROPERTY GROUP LIMITED</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16473543</t>
+          <t>16473525</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3867,7 +3859,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>56103</t>
+          <t>68100</t>
         </is>
       </c>
       <c r="J76" t="inlineStr"/>
@@ -3876,12 +3868,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>NIVADO SERVICES LIMITED</t>
+          <t>MJE FACILITIES CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16473521</t>
+          <t>16473821</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3912,7 +3904,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>41202</t>
+          <t>81100</t>
         </is>
       </c>
       <c r="J77" t="inlineStr"/>
@@ -3921,12 +3913,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>BOON AFRO-CARIBBEAN HAIR LOUNGE LTD</t>
+          <t>CRAWFORD HS LIMITED</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16473551</t>
+          <t>16473818</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3957,7 +3949,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>47789</t>
+          <t>74909</t>
         </is>
       </c>
       <c r="J78" t="inlineStr"/>
@@ -3966,12 +3958,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>JULIAN FRANCIS LTD</t>
+          <t>NA GLOBAL LIMITED</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16473523</t>
+          <t>16473758</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -4002,7 +3994,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>38320</t>
+          <t>41201,41202</t>
         </is>
       </c>
       <c r="J79" t="inlineStr"/>
@@ -4011,12 +4003,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>DAILY DASH STORE LIMITED</t>
+          <t>TAP &amp; WASH LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16473569</t>
+          <t>16473555</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -4047,7 +4039,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>47110</t>
+          <t>81299</t>
         </is>
       </c>
       <c r="J80" t="inlineStr"/>
@@ -4056,12 +4048,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>IACO PROPERTY LTD</t>
+          <t>SSMARTTEC LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>SC849759</t>
+          <t>16473466</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -4092,7 +4084,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>68100,68209</t>
+          <t>61200,62020</t>
         </is>
       </c>
       <c r="J81" t="inlineStr"/>
@@ -4101,12 +4093,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>AEVA MEDICAL LTD</t>
+          <t>WELCOME MART LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16473575</t>
+          <t>16473757</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -4137,7 +4129,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>86220,86900,96020</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J82" t="inlineStr"/>
@@ -4146,12 +4138,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>BURY LODGE FARM &amp; SERVICES LIMITED</t>
+          <t>MINI PRINT FACTORY LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16473568</t>
+          <t>16473759</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -4182,7 +4174,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>01300,01500</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J83" t="inlineStr"/>
@@ -4191,12 +4183,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>SAGA STUDIO LTD</t>
+          <t>MURRAY'S COFFEE LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16473564</t>
+          <t>16473717</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4227,7 +4219,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>74100</t>
+          <t>10832,56103,56210</t>
         </is>
       </c>
       <c r="J84" t="inlineStr"/>
@@ -4236,12 +4228,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>NOTHING SOUNDS GOOD LIMITED</t>
+          <t>R&amp;H KHUSHI LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16473566</t>
+          <t>16473718</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -4272,7 +4264,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>47630</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J85" t="inlineStr"/>
@@ -4281,12 +4273,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>WOW BUBBLES BARNSLEY LTD</t>
+          <t>ECOPOWER RENEWABLE SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16473572</t>
+          <t>SC849780</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -4317,7 +4309,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>56102</t>
+          <t>43210</t>
         </is>
       </c>
       <c r="J86" t="inlineStr"/>
@@ -4326,12 +4318,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ELMWOOD PROPERTY MANAGEMENT AND LETTINGS LIMITED</t>
+          <t>MZOF LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16473574</t>
+          <t>16473719</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -4362,7 +4354,7 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>68209,68320</t>
+          <t>59111</t>
         </is>
       </c>
       <c r="J87" t="inlineStr"/>
@@ -4371,12 +4363,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>HOUSE OF SAFFRON LIMITED</t>
+          <t>FHFC LIMITED</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16473645</t>
+          <t>16473652</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -4416,12 +4408,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>PITU BRICKWORK LTD</t>
+          <t>CLARITY HOME HUB HEALTH LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16473644</t>
+          <t>16473605</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -4452,7 +4444,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>41202</t>
+          <t>86900</t>
         </is>
       </c>
       <c r="J89" t="inlineStr"/>
@@ -4461,12 +4453,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>SELDUR LTD</t>
+          <t>SEVEN (HOLDCO) LIMITED</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16473642</t>
+          <t>16473606</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -4497,21 +4489,29 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>68209</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr"/>
-      <c r="K90" t="inlineStr"/>
+          <t>64209</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Activities of other holding companies n.e.c.</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>LATHAM INDUSTRIES (WEST MIDLANDS) LIMITED</t>
+          <t>EL RESALES LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16473643</t>
+          <t>SC849752</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -4542,7 +4542,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>31090</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J91" t="inlineStr"/>
@@ -4551,12 +4551,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>EN4 RESTAURANT LIMITED</t>
+          <t>RESOLUTIO CONSULTING LTD</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16473650</t>
+          <t>16473560</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -4587,7 +4587,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>56101</t>
+          <t>82990</t>
         </is>
       </c>
       <c r="J92" t="inlineStr"/>
@@ -4596,12 +4596,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>THE BUNKER LEVEN LIMITED</t>
+          <t>COMPASS HOUSING SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>SC849768</t>
+          <t>16473554</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -4632,7 +4632,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>56302</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J93" t="inlineStr"/>
@@ -4641,12 +4641,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>LAYLAH COUNSELLING LIMITED</t>
+          <t>ZENCRUITERS LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16473672</t>
+          <t>16473562</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4677,7 +4677,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>84120</t>
+          <t>78109</t>
         </is>
       </c>
       <c r="J94" t="inlineStr"/>
@@ -4686,12 +4686,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>ZEENUNGOS LIMITED</t>
+          <t>ROKSEE LIMITED</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16473674</t>
+          <t>16473563</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4722,7 +4722,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>87100</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J95" t="inlineStr"/>
@@ -4731,12 +4731,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>NFGU COACHING LTD</t>
+          <t>GLOBAL LETTING AND MAINTENANCE LTD</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16473802</t>
+          <t>16473561</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>93130</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J96" t="inlineStr"/>
@@ -4776,12 +4776,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>SDT GLOBAL SERVICES LTD</t>
+          <t>GANDER INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16473808</t>
+          <t>16473515</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4807,12 +4807,12 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>47190,69201,70229,71122</t>
+          <t>68100,68209</t>
         </is>
       </c>
       <c r="J97" t="inlineStr"/>
@@ -4821,12 +4821,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>RUGER CONSULTING LTD</t>
+          <t>HOLLY LARKHAM CARE LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16473547</t>
+          <t>16473517</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>87300</t>
         </is>
       </c>
       <c r="J98" t="inlineStr"/>
@@ -4866,12 +4866,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>ROUSE SHARP LTD</t>
+          <t>MIGHTY FORTRESS ESTATES LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16473550</t>
+          <t>16473513</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4902,7 +4902,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>41100,68209</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J99" t="inlineStr"/>
@@ -4911,12 +4911,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>DISTINGUISH SISTERS LIMITED LIMITED</t>
+          <t>VICTORY NINE LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16473470</t>
+          <t>16473475</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4947,7 +4947,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>84120,86900,87200</t>
+          <t>73110</t>
         </is>
       </c>
       <c r="J100" t="inlineStr"/>
@@ -4956,12 +4956,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>DELAN CUILEY LIMITED</t>
+          <t>HIGH STREET CORNER STORE LTD</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>NI729778</t>
+          <t>16473558</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4992,7 +4992,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>46210,46341,47910</t>
+          <t>47110</t>
         </is>
       </c>
       <c r="J101" t="inlineStr"/>
@@ -5001,12 +5001,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>ERSA MEDICAL UK LTD</t>
+          <t>MONCHERRI LTD</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>16473148</t>
+          <t>16473339</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -5037,7 +5037,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>46900,47749</t>
+          <t>14142,46420,47710</t>
         </is>
       </c>
       <c r="J102" t="inlineStr"/>
@@ -5046,12 +5046,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>NEXA CLEANING LTD</t>
+          <t>FINTHOS LTD</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>16473345</t>
+          <t>NI729773</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>81210</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J103" t="inlineStr"/>
@@ -5091,12 +5091,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>GREEN HILL ADVISORY LIMITED</t>
+          <t>NAILD LTD</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>16473162</t>
+          <t>16473286</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -5127,7 +5127,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>63120</t>
         </is>
       </c>
       <c r="J104" t="inlineStr"/>
@@ -5136,12 +5136,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ATLANTIS DESIGN LTD</t>
+          <t>THE WOMENS PT ACADEMY LIMITED</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>16473155</t>
+          <t>16473285</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -5172,7 +5172,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>47910,74100</t>
+          <t>85510</t>
         </is>
       </c>
       <c r="J105" t="inlineStr"/>
@@ -5181,12 +5181,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>RAVIEN PROPERTY LTD</t>
+          <t>ZARI TRAVELS LTD</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>16473210</t>
+          <t>16473080</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -5217,7 +5217,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>49320,79110</t>
         </is>
       </c>
       <c r="J106" t="inlineStr"/>
@@ -5226,12 +5226,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>AHED ABDEL HAMID LTD</t>
+          <t>HESSE HEATING LIMITED</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>16473226</t>
+          <t>16473431</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -5262,7 +5262,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>46900</t>
+          <t>43220</t>
         </is>
       </c>
       <c r="J107" t="inlineStr"/>
@@ -5271,12 +5271,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>S K Y LOUNGE COV LTD</t>
+          <t>ENLAB LIMITED</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>16473289</t>
+          <t>16473427</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -5307,7 +5307,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>56102</t>
+          <t>62020</t>
         </is>
       </c>
       <c r="J108" t="inlineStr"/>
@@ -5316,12 +5316,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>TQ HEALTH FITNESS AND WELL-BEING LTD</t>
+          <t>INTERCONTINENTAL HOLDING COMPANY LIMITED</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SC849740</t>
+          <t>16473418</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -5352,21 +5352,29 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>85510</t>
-        </is>
-      </c>
-      <c r="J109" t="inlineStr"/>
-      <c r="K109" t="inlineStr"/>
+          <t>64209</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>Activities of other holding companies n.e.c.</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>SILJENA LTD</t>
+          <t>AWEXIA LTD</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>16473291</t>
+          <t>16473430</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -5397,7 +5405,7 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>62090,73110,74100</t>
+          <t>47910,47990</t>
         </is>
       </c>
       <c r="J110" t="inlineStr"/>
@@ -5406,12 +5414,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>NASWILL HOMES LIMITED</t>
+          <t>SKILLS 4 CAREERS LTD</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>16473347</t>
+          <t>16473283</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -5442,7 +5450,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>68100,68209,68320</t>
+          <t>85590</t>
         </is>
       </c>
       <c r="J111" t="inlineStr"/>
@@ -5451,12 +5459,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>PINK PEGASUS BOOKSHOP LTD</t>
+          <t>MCPHILLIPS CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>16473346</t>
+          <t>SC849745</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -5487,7 +5495,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>47610</t>
+          <t>41201,41202,43999</t>
         </is>
       </c>
       <c r="J112" t="inlineStr"/>
@@ -5496,12 +5504,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>BOBBINS BAKES LIMITED</t>
+          <t>DN TRAINING LTD</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>16473350</t>
+          <t>16473154</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -5532,7 +5540,7 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>10920</t>
+          <t>85590</t>
         </is>
       </c>
       <c r="J113" t="inlineStr"/>
@@ -5541,12 +5549,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>NOAH PRO LTD</t>
+          <t>AMS CONSTRUCTION CHESHIRE LTD</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>16473344</t>
+          <t>16473282</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -5577,7 +5585,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>41202,43310,43910</t>
         </is>
       </c>
       <c r="J114" t="inlineStr"/>
@@ -5586,12 +5594,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>AAA PORTFOLIO LTD</t>
+          <t>TOBIN85 LTD</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>16473079</t>
+          <t>16473284</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -5622,7 +5630,7 @@
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>45200</t>
+          <t>53202</t>
         </is>
       </c>
       <c r="J115" t="inlineStr"/>
@@ -5631,12 +5639,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>DB HEALTH LTD</t>
+          <t>M DIAB LTD</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>16473401</t>
+          <t>16473153</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -5667,7 +5675,7 @@
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>65120</t>
+          <t>56101,56102,56290,56302</t>
         </is>
       </c>
       <c r="J116" t="inlineStr"/>
@@ -5676,12 +5684,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>HAUS OF HOUNDS LTD</t>
+          <t>MUM STUDIO LTD</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>16473404</t>
+          <t>16473150</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -5712,7 +5720,7 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>14190</t>
+          <t>47910,47990</t>
         </is>
       </c>
       <c r="J117" t="inlineStr"/>
@@ -5721,12 +5729,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>ALISHA ZANIB LTD</t>
+          <t>CM SUPERSTORE LTD</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>16473403</t>
+          <t>16473152</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -5757,7 +5765,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>47910,47990</t>
         </is>
       </c>
       <c r="J118" t="inlineStr"/>
@@ -5766,12 +5774,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>SR CASH AND CARRY LTD</t>
+          <t>TLJ INVESTMENT LTD</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>16473399</t>
+          <t>16473151</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -5797,12 +5805,12 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>46310,46390,46900,47250</t>
+          <t>41100,55100,68100</t>
         </is>
       </c>
       <c r="J119" t="inlineStr"/>
@@ -5811,12 +5819,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>RUNLATES LTD</t>
+          <t>CLEAN CULT LIMITED</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>16473402</t>
+          <t>16473120</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -5847,7 +5855,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>93130</t>
+          <t>81210</t>
         </is>
       </c>
       <c r="J120" t="inlineStr"/>
@@ -5856,12 +5864,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>LONDON DUUKA UK LTD</t>
+          <t>NAYCĦ COLLECTIVE LTD</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>16473044</t>
+          <t>16473119</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -5892,7 +5900,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>46160,47710,47820,47910</t>
         </is>
       </c>
       <c r="J121" t="inlineStr"/>
@@ -5901,12 +5909,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>STAGEPAPER LTD</t>
+          <t>VINED ME LTD</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>16473057</t>
+          <t>16473118</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -5937,7 +5945,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>82990</t>
+          <t>46342,47250</t>
         </is>
       </c>
       <c r="J122" t="inlineStr"/>
@@ -5946,12 +5954,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>METAL &amp; MYTH LTD</t>
+          <t>JETMAR PROPERTY &amp; SERVICES LTD</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>16473064</t>
+          <t>NI729770</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -5982,7 +5990,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>32120</t>
+          <t>68100,81210</t>
         </is>
       </c>
       <c r="J123" t="inlineStr"/>
@@ -5991,12 +5999,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>BA SELLERS LTD</t>
+          <t>LUX CATALOGUE LTD</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>16473060</t>
+          <t>16473367</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -6036,12 +6044,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>LOWENKRAFT LTD</t>
+          <t>GARDEN MAINTENANCE SERVICES LTD</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>16473061</t>
+          <t>16473369</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -6072,7 +6080,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>81300</t>
         </is>
       </c>
       <c r="J125" t="inlineStr"/>
@@ -6081,12 +6089,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>QUALITY AND COMPLIANCE CONSULTANCY SERVICES LTD</t>
+          <t>TMB SCAFFOLDING LTD</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>16473159</t>
+          <t>16473163</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -6117,7 +6125,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>43991</t>
         </is>
       </c>
       <c r="J126" t="inlineStr"/>
@@ -6126,12 +6134,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>DOMAINO6 LTD</t>
+          <t>CARYS PLANT LTD</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>16473156</t>
+          <t>16473056</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -6162,7 +6170,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>46900</t>
+          <t>86900</t>
         </is>
       </c>
       <c r="J127" t="inlineStr"/>
@@ -6171,12 +6179,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>KAYA SPECIALIST CARE LTD</t>
+          <t>KHEDMAT LTD</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>16473112</t>
+          <t>16473362</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -6207,7 +6215,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>86220</t>
+          <t>79110</t>
         </is>
       </c>
       <c r="J128" t="inlineStr"/>
@@ -6216,12 +6224,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>BLUEPRINT CONTENT STUDIOS LIMITED</t>
+          <t>RC RIGGERS LTD</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>16473116</t>
+          <t>16473048</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -6252,7 +6260,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>96090</t>
+          <t>90020</t>
         </is>
       </c>
       <c r="J129" t="inlineStr"/>
@@ -6261,12 +6269,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>BITSNBOBS THE 3D PRINT SHOP LTD</t>
+          <t>CWPG GROUNDWORKS LTD</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>16473137</t>
+          <t>16473363</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -6297,7 +6305,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>47789</t>
+          <t>81300</t>
         </is>
       </c>
       <c r="J130" t="inlineStr"/>
@@ -6306,12 +6314,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>BRIDGEWICK PARTNERS LIMITED</t>
+          <t>ELECTRIC SAFE LTD</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>16473142</t>
+          <t>16473300</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -6337,34 +6345,26 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>64999</t>
-        </is>
-      </c>
-      <c r="J131" t="inlineStr">
-        <is>
-          <t>Financial intermediation not elsewhere classified</t>
-        </is>
-      </c>
-      <c r="K131" t="inlineStr">
-        <is>
-          <t>Catch-all credit-oriented SPVs for novel lending structures.</t>
-        </is>
-      </c>
+          <t>43210,47540</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr"/>
+      <c r="K131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>THESAFETYSAVVY LTD</t>
+          <t>S SINGH BUILDER LTD</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>16473135</t>
+          <t>16473306</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>86900</t>
+          <t>41202</t>
         </is>
       </c>
       <c r="J132" t="inlineStr"/>
@@ -6404,12 +6404,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>RMS FINANCE CONSULTING LIMITED</t>
+          <t>PANADENT LTD</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>16473232</t>
+          <t>16473302</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -6440,7 +6440,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>86230</t>
         </is>
       </c>
       <c r="J133" t="inlineStr"/>
@@ -6449,12 +6449,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>LAMONT BUILDS LIMITED</t>
+          <t>FORSTER PRODUCTIONS LTD</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>16473230</t>
+          <t>16473303</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -6485,7 +6485,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>41201,41202,71111</t>
+          <t>90010</t>
         </is>
       </c>
       <c r="J134" t="inlineStr"/>
@@ -6494,12 +6494,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>MARMIMI HOLDING LIMITED</t>
+          <t>SILENTSTACKS LIMITED</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>16473234</t>
+          <t>16473308</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -6530,29 +6530,21 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>64209</t>
-        </is>
-      </c>
-      <c r="J135" t="inlineStr">
-        <is>
-          <t>Activities of other holding companies n.e.c.</t>
-        </is>
-      </c>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
-        </is>
-      </c>
+          <t>46190</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr"/>
+      <c r="K135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>HEALTH &amp; WELLNESS MEDICA CLINIC LTD</t>
+          <t>PAF PROPERTY LTD</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>16473242</t>
+          <t>16473259</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -6583,7 +6575,7 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>47730</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J136" t="inlineStr"/>
@@ -6592,12 +6584,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>JOHN HUGHES DECS LIMITED</t>
+          <t>THE PAINTMAN AUTO REPAIRS LTD</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>SC849734</t>
+          <t>16473256</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -6628,7 +6620,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>43341</t>
+          <t>45200</t>
         </is>
       </c>
       <c r="J137" t="inlineStr"/>
@@ -6637,12 +6629,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>GIGGLE GARDEN PLAY CAFE LTD</t>
+          <t>AIRPORT TR4NSPORT SPECI4LISTS LIMITED</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>16473294</t>
+          <t>16473263</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -6673,7 +6665,7 @@
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>56102,88910</t>
+          <t>49320</t>
         </is>
       </c>
       <c r="J138" t="inlineStr"/>
@@ -6682,12 +6674,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>BIKER GEARS LTD</t>
+          <t>GAUNT CAPITAL LTD</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>16473293</t>
+          <t>16473262</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -6713,26 +6705,34 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>45310,46420,47910</t>
-        </is>
-      </c>
-      <c r="J139" t="inlineStr"/>
-      <c r="K139" t="inlineStr"/>
+          <t>64209</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>Activities of other holding companies n.e.c.</t>
+        </is>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>TG BARGAIN LTD</t>
+          <t>CEDRIC PROPERTY LTD</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>16473326</t>
+          <t>SC849737</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -6763,7 +6763,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J140" t="inlineStr"/>
@@ -6772,12 +6772,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>PINK FLAMINGO HOLDINGS LIMITED</t>
+          <t>CASA DUNMAR LTD</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>16473327</t>
+          <t>SC849728</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -6817,12 +6817,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>AJ INVESTMENT AND CONSULTANCY LTD</t>
+          <t>RR DRAINAGE SERVICES LTD</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>16473328</t>
+          <t>16473164</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -6848,34 +6848,26 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>64306,70229</t>
-        </is>
-      </c>
-      <c r="J142" t="inlineStr">
-        <is>
-          <t>Activities of real estate investment trusts</t>
-        </is>
-      </c>
-      <c r="K142" t="inlineStr">
-        <is>
-          <t>UK-regulated REIT companies.</t>
-        </is>
-      </c>
+          <t>43999</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr"/>
+      <c r="K142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>THE MINDSHIFT METHOD LTD</t>
+          <t>RAQT SPORTS LTD</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>16473330</t>
+          <t>16473167</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -6906,7 +6898,7 @@
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>86900</t>
+          <t>47190</t>
         </is>
       </c>
       <c r="J143" t="inlineStr"/>
@@ -6915,12 +6907,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>RASTA REALTY LTD</t>
+          <t>UYR GOODS LIMITED</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>16473325</t>
+          <t>16473039</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -6951,7 +6943,7 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J144" t="inlineStr"/>
@@ -6960,12 +6952,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>ELITE PROPERTIES &amp; HOUSING LTD</t>
+          <t>SAINTS HALAL SUPERMARKET LIMITED</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>16473397</t>
+          <t>16473074</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -6996,7 +6988,7 @@
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>68100,68209,68320</t>
+          <t>47110,47190,47220</t>
         </is>
       </c>
       <c r="J145" t="inlineStr"/>
@@ -7005,12 +6997,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>PLATINUM MARKETING LONDON LTD</t>
+          <t>ACHILLE CONSTRUCTION SERVICE LTD</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>16473396</t>
+          <t>16473038</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -7041,7 +7033,7 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>70229,73110</t>
+          <t>82990</t>
         </is>
       </c>
       <c r="J146" t="inlineStr"/>
@@ -7050,12 +7042,12 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>THE DISLEY GROUP LTD</t>
+          <t>STUDIO11 CONTENT LTD</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>16473398</t>
+          <t>16473066</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -7086,29 +7078,21 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>64209</t>
-        </is>
-      </c>
-      <c r="J147" t="inlineStr">
-        <is>
-          <t>Activities of other holding companies n.e.c.</t>
-        </is>
-      </c>
-      <c r="K147" t="inlineStr">
-        <is>
-          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
-        </is>
-      </c>
+          <t>73110</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr"/>
+      <c r="K147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>AGC STEEL LIMITED</t>
+          <t>AMBERSTAR LANDSCAPES LTD</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>NI729774</t>
+          <t>16473052</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -7139,7 +7123,7 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>25110</t>
+          <t>71112</t>
         </is>
       </c>
       <c r="J148" t="inlineStr"/>
@@ -7148,12 +7132,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>NEUBO LTD</t>
+          <t>REVYN BEAUTY LTD</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>16473395</t>
+          <t>16473059</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -7184,7 +7168,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>47750</t>
         </is>
       </c>
       <c r="J149" t="inlineStr"/>
@@ -7193,12 +7177,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>ABC STUDIO CHILDCARE PLUS LTD</t>
+          <t>RENOPLUMB LTD</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>16473106</t>
+          <t>16473045</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -7229,7 +7213,7 @@
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>88910</t>
+          <t>41201,41202,43220</t>
         </is>
       </c>
       <c r="J150" t="inlineStr"/>
@@ -7238,12 +7222,12 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>HORIZON RESOURCING LTD</t>
+          <t>ERSA MEDICAL UK LTD</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>16473058</t>
+          <t>16473148</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -7274,7 +7258,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>78109</t>
+          <t>46900,47749</t>
         </is>
       </c>
       <c r="J151" t="inlineStr"/>
@@ -7283,12 +7267,12 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>RC RIGGERS LTD</t>
+          <t>HORIZON RESOURCING LTD</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>16473048</t>
+          <t>16473058</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -7319,7 +7303,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>90020</t>
+          <t>78109</t>
         </is>
       </c>
       <c r="J152" t="inlineStr"/>
@@ -7328,12 +7312,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>RENOPLUMB LTD</t>
+          <t>NOAH PRO LTD</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>16473045</t>
+          <t>16473344</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -7364,7 +7348,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>41201,41202,43220</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J153" t="inlineStr"/>
@@ -7373,12 +7357,12 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>MCPHILLIPS CONSTRUCTION LTD</t>
+          <t>BA SELLERS LTD</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>SC849745</t>
+          <t>16473060</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -7409,7 +7393,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>41201,41202,43999</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J154" t="inlineStr"/>
@@ -7418,12 +7402,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>JETMAR PROPERTY &amp; SERVICES LTD</t>
+          <t>METAL &amp; MYTH LTD</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>NI729770</t>
+          <t>16473064</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -7454,7 +7438,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>68100,81210</t>
+          <t>32120</t>
         </is>
       </c>
       <c r="J155" t="inlineStr"/>
@@ -7463,12 +7447,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>VINED ME LTD</t>
+          <t>STAGEPAPER LTD</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>16473118</t>
+          <t>16473057</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -7499,7 +7483,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>46342,47250</t>
+          <t>82990</t>
         </is>
       </c>
       <c r="J156" t="inlineStr"/>
@@ -7508,12 +7492,12 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>NAYCĦ COLLECTIVE LTD</t>
+          <t>LONDON DUUKA UK LTD</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>16473119</t>
+          <t>16473044</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -7544,7 +7528,7 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>46160,47710,47820,47910</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J157" t="inlineStr"/>
@@ -7553,12 +7537,12 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>CLEAN CULT LIMITED</t>
+          <t>RUNLATES LTD</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>16473120</t>
+          <t>16473402</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -7589,7 +7573,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>81210</t>
+          <t>93130</t>
         </is>
       </c>
       <c r="J158" t="inlineStr"/>
@@ -7598,12 +7582,12 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>TLJ INVESTMENT LTD</t>
+          <t>SR CASH AND CARRY LTD</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>16473151</t>
+          <t>16473399</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -7629,12 +7613,12 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>41100,55100,68100</t>
+          <t>46310,46390,46900,47250</t>
         </is>
       </c>
       <c r="J159" t="inlineStr"/>
@@ -7643,12 +7627,12 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>CM SUPERSTORE LTD</t>
+          <t>ALISHA ZANIB LTD</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>16473152</t>
+          <t>16473403</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -7679,7 +7663,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>47910,47990</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J160" t="inlineStr"/>
@@ -7688,12 +7672,12 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>DN TRAINING LTD</t>
+          <t>HAUS OF HOUNDS LTD</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>16473154</t>
+          <t>16473404</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -7724,7 +7708,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>85590</t>
+          <t>14190</t>
         </is>
       </c>
       <c r="J161" t="inlineStr"/>
@@ -7733,12 +7717,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>MUM STUDIO LTD</t>
+          <t>DB HEALTH LTD</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>16473150</t>
+          <t>16473401</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -7769,7 +7753,7 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>47910,47990</t>
+          <t>65120</t>
         </is>
       </c>
       <c r="J162" t="inlineStr"/>
@@ -7778,12 +7762,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>M DIAB LTD</t>
+          <t>AAA PORTFOLIO LTD</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>16473153</t>
+          <t>16473079</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -7814,7 +7798,7 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>56101,56102,56290,56302</t>
+          <t>45200</t>
         </is>
       </c>
       <c r="J163" t="inlineStr"/>
@@ -7823,12 +7807,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>TOBIN85 LTD</t>
+          <t>BOBBINS BAKES LIMITED</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>16473284</t>
+          <t>16473350</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -7859,7 +7843,7 @@
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>53202</t>
+          <t>10920</t>
         </is>
       </c>
       <c r="J164" t="inlineStr"/>
@@ -7868,12 +7852,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>AMS CONSTRUCTION CHESHIRE LTD</t>
+          <t>ABC STUDIO CHILDCARE PLUS LTD</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>16473282</t>
+          <t>16473106</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -7904,7 +7888,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>41202,43310,43910</t>
+          <t>88910</t>
         </is>
       </c>
       <c r="J165" t="inlineStr"/>
@@ -7913,12 +7897,12 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>SKILLS 4 CAREERS LTD</t>
+          <t>PINK PEGASUS BOOKSHOP LTD</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>16473283</t>
+          <t>16473346</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -7949,7 +7933,7 @@
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>85590</t>
+          <t>47610</t>
         </is>
       </c>
       <c r="J166" t="inlineStr"/>
@@ -7958,12 +7942,12 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>FINTHOS LTD</t>
+          <t>NASWILL HOMES LIMITED</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>NI729773</t>
+          <t>16473347</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -7994,7 +7978,7 @@
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>70229</t>
+          <t>68100,68209,68320</t>
         </is>
       </c>
       <c r="J167" t="inlineStr"/>
@@ -8003,12 +7987,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>NAILD LTD</t>
+          <t>SILJENA LTD</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>16473286</t>
+          <t>16473291</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -8039,7 +8023,7 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>63120</t>
+          <t>62090,73110,74100</t>
         </is>
       </c>
       <c r="J168" t="inlineStr"/>
@@ -8048,12 +8032,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>THE WOMENS PT ACADEMY LIMITED</t>
+          <t>TQ HEALTH FITNESS AND WELL-BEING LTD</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>16473285</t>
+          <t>SC849740</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -8093,12 +8077,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>MONCHERRI LTD</t>
+          <t>S K Y LOUNGE COV LTD</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>16473339</t>
+          <t>16473289</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -8129,7 +8113,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>14142,46420,47710</t>
+          <t>56102</t>
         </is>
       </c>
       <c r="J170" t="inlineStr"/>
@@ -8138,12 +8122,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>HESSE HEATING LIMITED</t>
+          <t>AHED ABDEL HAMID LTD</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>16473431</t>
+          <t>16473226</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -8174,7 +8158,7 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>43220</t>
+          <t>46900</t>
         </is>
       </c>
       <c r="J171" t="inlineStr"/>
@@ -8183,12 +8167,12 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>ENLAB LIMITED</t>
+          <t>RAVIEN PROPERTY LTD</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>16473427</t>
+          <t>16473210</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -8219,7 +8203,7 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>62020</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J172" t="inlineStr"/>
@@ -8228,12 +8212,12 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>INTERCONTINENTAL HOLDING COMPANY LIMITED</t>
+          <t>ATLANTIS DESIGN LTD</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>16473418</t>
+          <t>16473155</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -8264,29 +8248,21 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>64209</t>
-        </is>
-      </c>
-      <c r="J173" t="inlineStr">
-        <is>
-          <t>Activities of other holding companies n.e.c.</t>
-        </is>
-      </c>
-      <c r="K173" t="inlineStr">
-        <is>
-          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
-        </is>
-      </c>
+          <t>47910,74100</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr"/>
+      <c r="K173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>AWEXIA LTD</t>
+          <t>GREEN HILL ADVISORY LIMITED</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>16473430</t>
+          <t>16473162</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -8317,7 +8293,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>47910,47990</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J174" t="inlineStr"/>
@@ -8326,12 +8302,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>ZARI TRAVELS LTD</t>
+          <t>NEXA CLEANING LTD</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>16473080</t>
+          <t>16473345</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -8362,7 +8338,7 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>49320,79110</t>
+          <t>81210</t>
         </is>
       </c>
       <c r="J175" t="inlineStr"/>
@@ -8371,12 +8347,12 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>GARDEN MAINTENANCE SERVICES LTD</t>
+          <t>LOWENKRAFT LTD</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>16473369</t>
+          <t>16473061</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -8407,7 +8383,7 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>81300</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J176" t="inlineStr"/>
@@ -8416,12 +8392,12 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>LUX CATALOGUE LTD</t>
+          <t>QUALITY AND COMPLIANCE CONSULTANCY SERVICES LTD</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>16473367</t>
+          <t>16473159</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -8452,7 +8428,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J177" t="inlineStr"/>
@@ -8461,12 +8437,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>CARYS PLANT LTD</t>
+          <t>DOMAINO6 LTD</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>16473056</t>
+          <t>16473156</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -8497,7 +8473,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>86900</t>
+          <t>46900</t>
         </is>
       </c>
       <c r="J178" t="inlineStr"/>
@@ -8506,12 +8482,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>KHEDMAT LTD</t>
+          <t>KAYA SPECIALIST CARE LTD</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>16473362</t>
+          <t>16473112</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -8542,7 +8518,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>79110</t>
+          <t>86220</t>
         </is>
       </c>
       <c r="J179" t="inlineStr"/>
@@ -8551,12 +8527,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>REVYN BEAUTY LTD</t>
+          <t>NEUBO LTD</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>16473059</t>
+          <t>16473395</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -8587,7 +8563,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>47750</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J180" t="inlineStr"/>
@@ -8596,12 +8572,12 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>AMBERSTAR LANDSCAPES LTD</t>
+          <t>AGC STEEL LIMITED</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>16473052</t>
+          <t>NI729774</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -8632,7 +8608,7 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>71112</t>
+          <t>25110</t>
         </is>
       </c>
       <c r="J181" t="inlineStr"/>
@@ -8641,12 +8617,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>STUDIO11 CONTENT LTD</t>
+          <t>THE DISLEY GROUP LTD</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>16473066</t>
+          <t>16473398</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -8677,21 +8653,29 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>73110</t>
-        </is>
-      </c>
-      <c r="J182" t="inlineStr"/>
-      <c r="K182" t="inlineStr"/>
+          <t>64209</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>Activities of other holding companies n.e.c.</t>
+        </is>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>ACHILLE CONSTRUCTION SERVICE LTD</t>
+          <t>PLATINUM MARKETING LONDON LTD</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>16473038</t>
+          <t>16473396</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -8722,7 +8706,7 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>82990</t>
+          <t>70229,73110</t>
         </is>
       </c>
       <c r="J183" t="inlineStr"/>
@@ -8731,12 +8715,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>SAINTS HALAL SUPERMARKET LIMITED</t>
+          <t>ELITE PROPERTIES &amp; HOUSING LTD</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>16473074</t>
+          <t>16473397</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -8767,7 +8751,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>47110,47190,47220</t>
+          <t>68100,68209,68320</t>
         </is>
       </c>
       <c r="J184" t="inlineStr"/>
@@ -8776,12 +8760,12 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>UYR GOODS LIMITED</t>
+          <t>RASTA REALTY LTD</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>16473039</t>
+          <t>16473325</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -8812,7 +8796,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J185" t="inlineStr"/>
@@ -8821,12 +8805,12 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>RAQT SPORTS LTD</t>
+          <t>THE MINDSHIFT METHOD LTD</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>16473167</t>
+          <t>16473330</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -8857,7 +8841,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>47190</t>
+          <t>86900</t>
         </is>
       </c>
       <c r="J186" t="inlineStr"/>
@@ -8866,12 +8850,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>RR DRAINAGE SERVICES LTD</t>
+          <t>AJ INVESTMENT AND CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>16473164</t>
+          <t>16473328</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -8897,26 +8881,34 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>43999</t>
-        </is>
-      </c>
-      <c r="J187" t="inlineStr"/>
-      <c r="K187" t="inlineStr"/>
+          <t>64306,70229</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>Activities of real estate investment trusts</t>
+        </is>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>UK-regulated REIT companies.</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>TMB SCAFFOLDING LTD</t>
+          <t>PINK FLAMINGO HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>16473163</t>
+          <t>16473327</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -8947,7 +8939,7 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>43991</t>
+          <t>68209</t>
         </is>
       </c>
       <c r="J188" t="inlineStr"/>
@@ -8956,12 +8948,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>CASA DUNMAR LTD</t>
+          <t>TG BARGAIN LTD</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>SC849728</t>
+          <t>16473326</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -8992,7 +8984,7 @@
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>47910</t>
         </is>
       </c>
       <c r="J189" t="inlineStr"/>
@@ -9001,12 +8993,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>CEDRIC PROPERTY LTD</t>
+          <t>BIKER GEARS LTD</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>SC849737</t>
+          <t>16473293</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -9037,7 +9029,7 @@
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>68209</t>
+          <t>45310,46420,47910</t>
         </is>
       </c>
       <c r="J190" t="inlineStr"/>
@@ -9046,12 +9038,12 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>GAUNT CAPITAL LTD</t>
+          <t>GIGGLE GARDEN PLAY CAFE LTD</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>16473262</t>
+          <t>16473294</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -9077,34 +9069,26 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>64209</t>
-        </is>
-      </c>
-      <c r="J191" t="inlineStr">
-        <is>
-          <t>Activities of other holding companies n.e.c.</t>
-        </is>
-      </c>
-      <c r="K191" t="inlineStr">
-        <is>
-          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
-        </is>
-      </c>
+          <t>56102,88910</t>
+        </is>
+      </c>
+      <c r="J191" t="inlineStr"/>
+      <c r="K191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>AIRPORT TR4NSPORT SPECI4LISTS LIMITED</t>
+          <t>JOHN HUGHES DECS LIMITED</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>16473263</t>
+          <t>SC849734</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -9135,7 +9119,7 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>49320</t>
+          <t>43341</t>
         </is>
       </c>
       <c r="J192" t="inlineStr"/>
@@ -9144,12 +9128,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>THE PAINTMAN AUTO REPAIRS LTD</t>
+          <t>HEALTH &amp; WELLNESS MEDICA CLINIC LTD</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>16473256</t>
+          <t>16473242</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -9180,7 +9164,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>45200</t>
+          <t>47730</t>
         </is>
       </c>
       <c r="J193" t="inlineStr"/>
@@ -9189,12 +9173,12 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>PAF PROPERTY LTD</t>
+          <t>MARMIMI HOLDING LIMITED</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>16473259</t>
+          <t>16473234</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -9225,21 +9209,29 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>68209</t>
-        </is>
-      </c>
-      <c r="J194" t="inlineStr"/>
-      <c r="K194" t="inlineStr"/>
+          <t>64209</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>Activities of other holding companies n.e.c.</t>
+        </is>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>Catch-all SPV: protected cells, cell companies, bespoke feeder vehicles.</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>SILENTSTACKS LIMITED</t>
+          <t>LAMONT BUILDS LIMITED</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>16473308</t>
+          <t>16473230</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -9270,7 +9262,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>46190</t>
+          <t>41201,41202,71111</t>
         </is>
       </c>
       <c r="J195" t="inlineStr"/>
@@ -9279,12 +9271,12 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>FORSTER PRODUCTIONS LTD</t>
+          <t>RMS FINANCE CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>16473303</t>
+          <t>16473232</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -9315,7 +9307,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>90010</t>
+          <t>70229</t>
         </is>
       </c>
       <c r="J196" t="inlineStr"/>
@@ -9324,12 +9316,12 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>PANADENT LTD</t>
+          <t>THESAFETYSAVVY LTD</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>16473302</t>
+          <t>16473135</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -9360,7 +9352,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>86230</t>
+          <t>86900</t>
         </is>
       </c>
       <c r="J197" t="inlineStr"/>
@@ -9369,12 +9361,12 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>S SINGH BUILDER LTD</t>
+          <t>BRIDGEWICK PARTNERS LIMITED</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>16473306</t>
+          <t>16473142</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -9400,26 +9392,34 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>41202</t>
-        </is>
-      </c>
-      <c r="J198" t="inlineStr"/>
-      <c r="K198" t="inlineStr"/>
+          <t>64999</t>
+        </is>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>Financial intermediation not elsewhere classified</t>
+        </is>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>Catch-all credit-oriented SPVs for novel lending structures.</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>ELECTRIC SAFE LTD</t>
+          <t>BITSNBOBS THE 3D PRINT SHOP LTD</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>16473300</t>
+          <t>16473137</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -9450,7 +9450,7 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>43210,47540</t>
+          <t>47789</t>
         </is>
       </c>
       <c r="J199" t="inlineStr"/>
@@ -9459,12 +9459,12 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>CWPG GROUNDWORKS LTD</t>
+          <t>BLUEPRINT CONTENT STUDIOS LIMITED</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>16473363</t>
+          <t>16473116</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -9495,7 +9495,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>81300</t>
+          <t>96090</t>
         </is>
       </c>
       <c r="J200" t="inlineStr"/>

</xml_diff>

<commit_message>
Stage 1: update companies data & retry manifest
</commit_message>
<xml_diff>
--- a/docs/assets/data/master_companies.xlsx
+++ b/docs/assets/data/master_companies.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Company Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Incorporation Date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Date Downloaded</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Time Discovered</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>SIC Codes</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SIC Description</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Typical Use Case</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>